<commit_message>
custom tpr_fpr that only use prominence
</commit_message>
<xml_diff>
--- a/practicum-experiment.xlsx
+++ b/practicum-experiment.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>TD</t>
   </si>
@@ -41,29 +41,62 @@
     <t xml:space="preserve">alpha settings </t>
   </si>
   <si>
-    <t>intermedia fd = 10</t>
-  </si>
-  <si>
     <t>beta settings</t>
   </si>
   <si>
-    <t>origin</t>
-  </si>
-  <si>
-    <t>rerun-1</t>
-  </si>
-  <si>
-    <t>return-2</t>
-  </si>
-  <si>
-    <t>Rerun-1</t>
+    <t>avg +- std</t>
+  </si>
+  <si>
+    <t>0.5251 +- 0.00272</t>
+  </si>
+  <si>
+    <t>0.6454 +- 0.031</t>
+  </si>
+  <si>
+    <t>0.6374 +- 0.028</t>
+  </si>
+  <si>
+    <t>0.5245 +- 0.005</t>
+  </si>
+  <si>
+    <t>0.6144 +- 0.0073</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>jump mean</t>
+  </si>
+  <si>
+    <t>HASC-2011</t>
+  </si>
+  <si>
+    <t>0.86 +- 0.01</t>
+  </si>
+  <si>
+    <t>0.9069 +- 0.02</t>
+  </si>
+  <si>
+    <t>0.9129 +- 0.018</t>
+  </si>
+  <si>
+    <t>0.9119 +- 0.017</t>
+  </si>
+  <si>
+    <t>0.8471 +- 0.02</t>
+  </si>
+  <si>
+    <t>0.8439 +- 0.048</t>
+  </si>
+  <si>
+    <t>0.859 +- 0.0136</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,16 +104,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -88,14 +133,95 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -374,142 +500,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A2:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.05078125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.05078125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.41660000000000003</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.65039999999999998</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.61719999999999997</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="5"/>
+      <c r="B10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.4284</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.86</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.62609999999999999</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0.877</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.62580000000000002</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0.41660000000000003</v>
-      </c>
-      <c r="C3">
-        <v>0.52329999999999999</v>
-      </c>
-      <c r="D3">
-        <v>5256</v>
-      </c>
-      <c r="F3">
-        <v>5290</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0.65039999999999998</v>
-      </c>
-      <c r="C4">
-        <v>0.63229999999999997</v>
-      </c>
-      <c r="D4">
-        <v>6273</v>
-      </c>
-      <c r="F4">
-        <v>5897</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I22">
         <v>1</v>
       </c>
-      <c r="B5">
-        <v>0.61719999999999997</v>
-      </c>
-      <c r="C5">
-        <v>0.6179</v>
-      </c>
-      <c r="D5">
-        <v>6218</v>
-      </c>
-      <c r="F5">
-        <v>6020</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>0.4284</v>
-      </c>
-      <c r="C9">
-        <v>0.52710000000000001</v>
-      </c>
-      <c r="D9">
-        <v>0.52710000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>0.62609999999999999</v>
-      </c>
-      <c r="C10">
-        <v>0.63319999999999999</v>
-      </c>
-      <c r="D10">
-        <v>0.63290000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>0.62580000000000002</v>
-      </c>
-      <c r="C11">
-        <v>0.62390000000000001</v>
-      </c>
-      <c r="D11">
-        <v>0.628</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add some dmd experiments with eeg dataset
</commit_message>
<xml_diff>
--- a/practicum-experiment.xlsx
+++ b/practicum-experiment.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="40">
   <si>
     <t>TD</t>
   </si>
@@ -195,6 +195,57 @@
   </si>
   <si>
     <t>EEG dataset</t>
+  </si>
+  <si>
+    <t>Method 5: DMD with svd=3, choose mode 0, label = 3 events</t>
+  </si>
+  <si>
+    <t>Method 6: DMD with svd=3, choose mode 0, label = 6 events</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: DMD, svd=1, labels=6</t>
+    </r>
+  </si>
+  <si>
+    <t>Method 8: svd=3, l2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method 9: ICA -&gt; DMD, svd = 1
+</t>
+  </si>
+  <si>
+    <t>Method 10: ICA -&gt; DMD, svd = 3, -&gt; L2</t>
+  </si>
+  <si>
+    <t>find a way to clean eeg data before put it in ICA or DMD</t>
+  </si>
+  <si>
+    <t>original code, (L2 only)</t>
+  </si>
+  <si>
+    <t>Method 7: dmd, svd=3 Look at each di.mensions</t>
+  </si>
+  <si>
+    <t>Method 7: dmd, svd=3 Look at each dimensions</t>
   </si>
 </sst>
 </file>
@@ -253,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -317,12 +368,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -356,8 +427,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -640,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -656,22 +743,23 @@
     <col min="7" max="7" width="15.1015625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.26171875" customWidth="1"/>
     <col min="9" max="9" width="14.41796875" customWidth="1"/>
+    <col min="13" max="13" width="14.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="G1" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="21" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-    </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="E3" s="7" t="s">
@@ -693,8 +781,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -725,8 +813,8 @@
         <v>0.4168</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="20"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="26"/>
       <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
@@ -755,8 +843,8 @@
         <v>0.55630000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="26"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
@@ -785,11 +873,11 @@
         <v>0.55479999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="26" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -817,8 +905,8 @@
         <v>0.60170000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="20"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="26"/>
       <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
@@ -844,8 +932,8 @@
         <v>0.43080000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="20"/>
+    <row r="10" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="26"/>
       <c r="B10" s="13" t="s">
         <v>1</v>
       </c>
@@ -871,12 +959,12 @@
         <v>0.59960000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:16" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="E16" s="7" t="s">
         <v>16</v>
       </c>
@@ -893,11 +981,29 @@
         <v>20</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="P16" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="26" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -909,11 +1015,33 @@
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="10"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="20"/>
+      <c r="I17" s="2">
+        <v>0.3982</v>
+      </c>
+      <c r="J17" s="24">
+        <v>0.4879</v>
+      </c>
+      <c r="K17" s="22">
+        <v>0.4506</v>
+      </c>
+      <c r="L17" s="22">
+        <v>0.47070000000000001</v>
+      </c>
+      <c r="M17" s="22">
+        <v>0.41770000000000002</v>
+      </c>
+      <c r="N17" s="25">
+        <v>0.50819999999999999</v>
+      </c>
+      <c r="O17" s="22">
+        <v>0.45479999999999998</v>
+      </c>
+      <c r="P17" s="22">
+        <v>0.41470000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="26"/>
       <c r="B18" s="12" t="s">
         <v>2</v>
       </c>
@@ -923,11 +1051,33 @@
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-    </row>
-    <row r="19" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="20"/>
+      <c r="I18" s="10">
+        <v>0.37880000000000003</v>
+      </c>
+      <c r="J18" s="24">
+        <v>0.48159999999999997</v>
+      </c>
+      <c r="K18" s="22">
+        <v>0.43630000000000002</v>
+      </c>
+      <c r="L18" s="22">
+        <v>0.46429999999999999</v>
+      </c>
+      <c r="M18" s="22">
+        <v>0.39290000000000003</v>
+      </c>
+      <c r="N18" s="25">
+        <v>0.48980000000000001</v>
+      </c>
+      <c r="O18" s="22">
+        <v>0.4355</v>
+      </c>
+      <c r="P18" s="22">
+        <v>0.41760000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A19" s="26"/>
       <c r="B19" s="13" t="s">
         <v>1</v>
       </c>
@@ -937,8 +1087,35 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="10"/>
+      <c r="I19" s="2">
+        <v>0.38829999999999998</v>
+      </c>
+      <c r="J19" s="24">
+        <v>0.48530000000000001</v>
+      </c>
+      <c r="K19" s="22">
+        <v>0.44169999999999998</v>
+      </c>
+      <c r="L19" s="22">
+        <v>0.46179999999999999</v>
+      </c>
+      <c r="M19" s="22">
+        <v>0.43540000000000001</v>
+      </c>
+      <c r="N19" s="25">
+        <v>0.46960000000000002</v>
+      </c>
+      <c r="O19" s="22">
+        <v>0.45119999999999999</v>
+      </c>
+      <c r="P19" s="22">
+        <v>0.41930000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -954,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="E6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -970,22 +1147,23 @@
     <col min="7" max="7" width="15.1015625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.26171875" customWidth="1"/>
     <col min="9" max="9" width="14.41796875" customWidth="1"/>
+    <col min="13" max="13" width="12.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="G1" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="21" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-    </row>
-    <row r="3" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="E3" s="7" t="s">
@@ -1007,8 +1185,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -1039,8 +1217,8 @@
         <v>0.59519999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="20"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="26"/>
       <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
@@ -1069,8 +1247,8 @@
         <v>0.6865</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="20"/>
+    <row r="6" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="26"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
@@ -1099,11 +1277,11 @@
         <v>0.68489999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="26" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1120,8 +1298,8 @@
       <c r="G8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="20"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="26"/>
       <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
@@ -1137,8 +1315,8 @@
       <c r="H9" s="10"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="20"/>
+    <row r="10" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="26"/>
       <c r="B10" s="13" t="s">
         <v>1</v>
       </c>
@@ -1154,19 +1332,199 @@
       <c r="H10" s="10"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="E16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="P16" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.5514</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2">
+        <v>0.51739999999999997</v>
+      </c>
+      <c r="J17" s="24">
+        <v>0.56910000000000005</v>
+      </c>
+      <c r="K17" s="22">
+        <v>0.56659999999999999</v>
+      </c>
+      <c r="L17" s="25">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="M17" s="22">
+        <v>0.51519999999999999</v>
+      </c>
+      <c r="N17" s="22">
+        <v>0.55859999999999999</v>
+      </c>
+      <c r="O17" s="22">
+        <v>0.55059999999999998</v>
+      </c>
+      <c r="P17" s="22">
+        <v>0.51519999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="26"/>
+      <c r="B18" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.54249999999999998</v>
+      </c>
+      <c r="G18" s="19"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="J18" s="19">
+        <v>0.57489999999999997</v>
+      </c>
+      <c r="K18" s="22">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="L18" s="22">
+        <v>0.55869999999999997</v>
+      </c>
+      <c r="M18" s="22">
+        <v>0.53159999999999996</v>
+      </c>
+      <c r="N18" s="22">
+        <v>0.54859999999999998</v>
+      </c>
+      <c r="O18" s="22">
+        <v>0.53680000000000005</v>
+      </c>
+      <c r="P18" s="22">
+        <v>0.53159999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A19" s="26"/>
+      <c r="B19" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2">
+        <v>0.52239999999999998</v>
+      </c>
+      <c r="J19" s="23">
+        <v>0.57709999999999995</v>
+      </c>
+      <c r="K19" s="22">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L19" s="22">
+        <v>0.57330000000000003</v>
+      </c>
+      <c r="M19" s="22">
+        <v>0.52170000000000005</v>
+      </c>
+      <c r="N19" s="22">
+        <v>0.55479999999999996</v>
+      </c>
+      <c r="O19" s="22">
+        <v>0.5524</v>
+      </c>
+      <c r="P19" s="22">
+        <v>0.52170000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="G2:J2"/>
+    <mergeCell ref="A17:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
change batch_size to 128
</commit_message>
<xml_diff>
--- a/practicum-experiment.xlsx
+++ b/practicum-experiment.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="41">
   <si>
     <t>TD</t>
   </si>
@@ -191,16 +191,10 @@
     <t>No report</t>
   </si>
   <si>
-    <t>original code, L2 norm, reproduce</t>
-  </si>
-  <si>
-    <t>EEG dataset</t>
-  </si>
-  <si>
     <t>Method 5: DMD with svd=3, choose mode 0, label = 3 events</t>
   </si>
   <si>
-    <t>Method 6: DMD with svd=3, choose mode 0, label = 6 events</t>
+    <t>find a way to clean eeg data before put it in ICA or DMD</t>
   </si>
   <si>
     <r>
@@ -212,6 +206,99 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Method 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ICA -&gt; L2 norm </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: DMD, svd=1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dmd, svd=3 -&gt; Look at each dimensions -&gt; combine CP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ICA -&gt; DMD, svd = 1
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Method 4</t>
     </r>
     <r>
@@ -222,30 +309,86 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: DMD, svd=1, labels=6</t>
-    </r>
-  </si>
-  <si>
-    <t>Method 8: svd=3, l2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Method 9: ICA -&gt; DMD, svd = 1
-</t>
-  </si>
-  <si>
-    <t>Method 10: ICA -&gt; DMD, svd = 3, -&gt; L2</t>
-  </si>
-  <si>
-    <t>find a way to clean eeg data before put it in ICA or DMD</t>
-  </si>
-  <si>
-    <t>original code, (L2 only)</t>
-  </si>
-  <si>
-    <t>Method 7: dmd, svd=3 Look at each di.mensions</t>
-  </si>
-  <si>
-    <t>Method 7: dmd, svd=3 Look at each dimensions</t>
+      <t>: ICA -&gt; DMD, svd = 3 -&gt; L2 norm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method 6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: DMD with svd=3, choose mode 0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method 7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: DMD, svd=3 -&gt; L2 norm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>original code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> L2 norm</t>
+    </r>
+  </si>
+  <si>
+    <t>EEG dataset, AUC score</t>
+  </si>
+  <si>
+    <t>EEG dataset, F1 score</t>
+  </si>
+  <si>
+    <t>Max</t>
   </si>
 </sst>
 </file>
@@ -304,7 +447,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -379,21 +522,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -419,32 +553,25 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -727,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -744,22 +871,23 @@
     <col min="8" max="8" width="15.26171875" customWidth="1"/>
     <col min="9" max="9" width="14.41796875" customWidth="1"/>
     <col min="13" max="13" width="14.734375" customWidth="1"/>
+    <col min="19" max="19" width="17.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="G1" s="18" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="27" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-    </row>
-    <row r="3" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="E3" s="7" t="s">
@@ -781,8 +909,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="24" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -813,8 +941,8 @@
         <v>0.4168</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="26"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="24"/>
       <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
@@ -843,8 +971,8 @@
         <v>0.55630000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="26"/>
+    <row r="6" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="24"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
@@ -873,11 +1001,11 @@
         <v>0.55479999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="24" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -905,8 +1033,8 @@
         <v>0.60170000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="26"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="24"/>
       <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
@@ -932,8 +1060,8 @@
         <v>0.43080000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="26"/>
+    <row r="10" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="24"/>
       <c r="B10" s="13" t="s">
         <v>1</v>
       </c>
@@ -959,170 +1087,189 @@
         <v>0.59960000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F15" t="s">
+    <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="83.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="S16" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2">
+        <v>0.41949999999999998</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0.41770000000000002</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.3982</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0.45479999999999998</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0.41470000000000001</v>
+      </c>
+      <c r="J17" s="22">
+        <v>0.4879</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0.47070000000000001</v>
+      </c>
+      <c r="L17" s="21">
+        <v>0.50819999999999999</v>
+      </c>
+      <c r="M17">
+        <f>MAX(E17:L17)</f>
+        <v>0.50819999999999999</v>
+      </c>
+      <c r="S17" s="20">
+        <v>0.4506</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="24"/>
+      <c r="B18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2">
+        <v>0.4199</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0.39290000000000003</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0.37880000000000003</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0.4355</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.41760000000000003</v>
+      </c>
+      <c r="J18" s="22">
+        <v>0.48159999999999997</v>
+      </c>
+      <c r="K18" s="10">
+        <v>0.46429999999999999</v>
+      </c>
+      <c r="L18" s="21">
+        <v>0.48980000000000001</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18:M19" si="0">MAX(E18:L18)</f>
+        <v>0.48980000000000001</v>
+      </c>
+      <c r="S18" s="20">
+        <v>0.43630000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="24"/>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0.43540000000000001</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.38829999999999998</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0.45119999999999999</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0.41930000000000001</v>
+      </c>
+      <c r="J19" s="21">
+        <v>0.48530000000000001</v>
+      </c>
+      <c r="K19" s="10">
+        <v>0.46179999999999999</v>
+      </c>
+      <c r="L19" s="22">
+        <v>0.46960000000000002</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>0.48530000000000001</v>
+      </c>
+      <c r="S19" s="20">
+        <v>0.44169999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="E16" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K16" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="L16" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="M16" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="N16" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="O16" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="P16" s="29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="2">
-        <v>0.41949999999999998</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2">
-        <v>0.3982</v>
-      </c>
-      <c r="J17" s="24">
-        <v>0.4879</v>
-      </c>
-      <c r="K17" s="22">
-        <v>0.4506</v>
-      </c>
-      <c r="L17" s="22">
-        <v>0.47070000000000001</v>
-      </c>
-      <c r="M17" s="22">
-        <v>0.41770000000000002</v>
-      </c>
-      <c r="N17" s="25">
-        <v>0.50819999999999999</v>
-      </c>
-      <c r="O17" s="22">
-        <v>0.45479999999999998</v>
-      </c>
-      <c r="P17" s="22">
-        <v>0.41470000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="26"/>
-      <c r="B18" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="2">
-        <v>0.4199</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="10">
-        <v>0.37880000000000003</v>
-      </c>
-      <c r="J18" s="24">
-        <v>0.48159999999999997</v>
-      </c>
-      <c r="K18" s="22">
-        <v>0.43630000000000002</v>
-      </c>
-      <c r="L18" s="22">
-        <v>0.46429999999999999</v>
-      </c>
-      <c r="M18" s="22">
-        <v>0.39290000000000003</v>
-      </c>
-      <c r="N18" s="25">
-        <v>0.48980000000000001</v>
-      </c>
-      <c r="O18" s="22">
-        <v>0.4355</v>
-      </c>
-      <c r="P18" s="22">
-        <v>0.41760000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="26"/>
-      <c r="B19" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6">
-        <v>0.39900000000000002</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2">
-        <v>0.38829999999999998</v>
-      </c>
-      <c r="J19" s="24">
-        <v>0.48530000000000001</v>
-      </c>
-      <c r="K19" s="22">
-        <v>0.44169999999999998</v>
-      </c>
-      <c r="L19" s="22">
-        <v>0.46179999999999999</v>
-      </c>
-      <c r="M19" s="22">
-        <v>0.43540000000000001</v>
-      </c>
-      <c r="N19" s="25">
-        <v>0.46960000000000002</v>
-      </c>
-      <c r="O19" s="22">
-        <v>0.45119999999999999</v>
-      </c>
-      <c r="P19" s="22">
-        <v>0.41930000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1131,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView topLeftCell="E6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1150,20 +1297,20 @@
     <col min="13" max="13" width="12.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="G1" s="18" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="27" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-    </row>
-    <row r="3" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="E3" s="7" t="s">
@@ -1185,8 +1332,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="24" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -1217,8 +1364,8 @@
         <v>0.59519999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="26"/>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="24"/>
       <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
@@ -1234,7 +1381,7 @@
       <c r="F5" s="2">
         <v>0.69689999999999996</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="18">
         <v>0.72199999999999998</v>
       </c>
       <c r="H5" s="9">
@@ -1247,8 +1394,8 @@
         <v>0.6865</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="26"/>
+    <row r="6" spans="1:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="24"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
@@ -1277,11 +1424,11 @@
         <v>0.68489999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="24" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1298,8 +1445,8 @@
       <c r="G8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="26"/>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="24"/>
       <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
@@ -1315,8 +1462,8 @@
       <c r="H9" s="10"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="26"/>
+    <row r="10" spans="1:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A10" s="24"/>
       <c r="B10" s="13" t="s">
         <v>1</v>
       </c>
@@ -1332,199 +1479,189 @@
       <c r="H10" s="10"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="E16" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="20" t="s">
+    <row r="15" spans="1:17" ht="27.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+    </row>
+    <row r="16" spans="1:17" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="23" t="s">
         <v>37</v>
       </c>
+      <c r="F16" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="G16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>21</v>
+        <v>30</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>33</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K16" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="L16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M16" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="N16" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="O16" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="P16" s="29" t="s">
+      <c r="K16" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="26" t="s">
+      <c r="L16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q16" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2">
         <v>0.5514</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2">
+      <c r="F17" s="10">
+        <v>0.51519999999999999</v>
+      </c>
+      <c r="G17" s="2">
         <v>0.51739999999999997</v>
       </c>
-      <c r="J17" s="24">
+      <c r="H17" s="10">
+        <v>0.55059999999999998</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0.51519999999999999</v>
+      </c>
+      <c r="J17" s="22">
         <v>0.56910000000000005</v>
       </c>
-      <c r="K17" s="22">
+      <c r="K17" s="21">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="L17" s="10">
+        <v>0.55859999999999999</v>
+      </c>
+      <c r="M17">
+        <f>MAX(E17:L17)</f>
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="Q17" s="20">
         <v>0.56659999999999999</v>
       </c>
-      <c r="L17" s="25">
-        <v>0.58499999999999996</v>
-      </c>
-      <c r="M17" s="22">
-        <v>0.51519999999999999</v>
-      </c>
-      <c r="N17" s="22">
-        <v>0.55859999999999999</v>
-      </c>
-      <c r="O17" s="22">
-        <v>0.55059999999999998</v>
-      </c>
-      <c r="P17" s="22">
-        <v>0.51519999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="26"/>
-      <c r="B18" s="12" t="s">
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="24"/>
+      <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2">
         <v>0.54249999999999998</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="H18" s="9"/>
+      <c r="F18" s="10">
+        <v>0.53159999999999996</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0.53680000000000005</v>
+      </c>
       <c r="I18" s="10">
-        <v>0.51400000000000001</v>
-      </c>
-      <c r="J18" s="19">
+        <v>0.53159999999999996</v>
+      </c>
+      <c r="J18" s="18">
         <v>0.57489999999999997</v>
       </c>
-      <c r="K18" s="22">
+      <c r="K18" s="10">
+        <v>0.55869999999999997</v>
+      </c>
+      <c r="L18" s="10">
+        <v>0.54859999999999998</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18:M19" si="0">MAX(E18:L18)</f>
+        <v>0.57489999999999997</v>
+      </c>
+      <c r="Q18" s="20">
         <v>0.54200000000000004</v>
       </c>
-      <c r="L18" s="22">
-        <v>0.55869999999999997</v>
-      </c>
-      <c r="M18" s="22">
-        <v>0.53159999999999996</v>
-      </c>
-      <c r="N18" s="22">
-        <v>0.54859999999999998</v>
-      </c>
-      <c r="O18" s="22">
-        <v>0.53680000000000005</v>
-      </c>
-      <c r="P18" s="22">
-        <v>0.53159999999999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A19" s="26"/>
-      <c r="B19" s="13" t="s">
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="24"/>
+      <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="6">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2">
         <v>0.54500000000000004</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2">
+      <c r="F19" s="10">
+        <v>0.52170000000000005</v>
+      </c>
+      <c r="G19" s="2">
         <v>0.52239999999999998</v>
       </c>
-      <c r="J19" s="23">
+      <c r="H19" s="10">
+        <v>0.5524</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0.52170000000000005</v>
+      </c>
+      <c r="J19" s="21">
         <v>0.57709999999999995</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="10">
+        <v>0.57330000000000003</v>
+      </c>
+      <c r="L19" s="10">
+        <v>0.55479999999999996</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>0.57709999999999995</v>
+      </c>
+      <c r="Q19" s="20">
         <v>0.56000000000000005</v>
       </c>
-      <c r="L19" s="22">
-        <v>0.57330000000000003</v>
-      </c>
-      <c r="M19" s="22">
-        <v>0.52170000000000005</v>
-      </c>
-      <c r="N19" s="22">
-        <v>0.55479999999999996</v>
-      </c>
-      <c r="O19" s="22">
-        <v>0.5524</v>
-      </c>
-      <c r="P19" s="22">
-        <v>0.52170000000000005</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix bug: eeg dataset produce change point error
</commit_message>
<xml_diff>
--- a/practicum-experiment.xlsx
+++ b/practicum-experiment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AUC" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="53">
   <si>
     <t>TD</t>
   </si>
@@ -389,6 +389,42 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>Original Code, L2</t>
+  </si>
+  <si>
+    <t>Dataset 1</t>
+  </si>
+  <si>
+    <t>Dataset 2</t>
+  </si>
+  <si>
+    <t>Dataset 3</t>
+  </si>
+  <si>
+    <t>Dataset 4</t>
+  </si>
+  <si>
+    <t>Dataset 5</t>
+  </si>
+  <si>
+    <t>Dataset 6</t>
+  </si>
+  <si>
+    <t>Dataset 7</t>
+  </si>
+  <si>
+    <t>Dataset 8</t>
+  </si>
+  <si>
+    <t>Method 5: DMD, svd = 1</t>
+  </si>
+  <si>
+    <t>Method 7: DMD, svd=3 -&gt; L2 norm</t>
+  </si>
+  <si>
+    <t>training: subject 1-&gt; 8 / validation: 9, 10 / testing: 11, 12. But now, only use training and testing set</t>
   </si>
 </sst>
 </file>
@@ -527,7 +563,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -565,13 +601,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -854,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:L15"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -880,12 +919,12 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
@@ -910,7 +949,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -942,7 +981,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
@@ -972,7 +1011,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
@@ -1005,7 +1044,7 @@
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="25" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1034,7 +1073,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
@@ -1061,7 +1100,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="24"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="13" t="s">
         <v>1</v>
       </c>
@@ -1088,20 +1127,20 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
       <c r="M15" t="s">
         <v>40</v>
       </c>
@@ -1120,7 +1159,7 @@
       <c r="G16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="24" t="s">
         <v>33</v>
       </c>
       <c r="I16" s="8" t="s">
@@ -1140,7 +1179,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1181,7 +1220,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="24"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
@@ -1220,7 +1259,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="24"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1263,8 +1302,313 @@
         <v>29</v>
       </c>
     </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2">
+        <v>0.36648999999999998</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="25"/>
+      <c r="B29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
+        <v>0.34767999999999999</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="25"/>
+      <c r="B30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2">
+        <v>0.36029</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="25"/>
+      <c r="B36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="25"/>
+      <c r="B37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="25"/>
+      <c r="B43" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="25"/>
+      <c r="B44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="11">
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A33:L33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A40:L40"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="G2:J2"/>
@@ -1278,10 +1622,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1303,12 +1647,12 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
@@ -1333,7 +1677,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -1365,7 +1709,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
@@ -1395,7 +1739,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
@@ -1428,7 +1772,7 @@
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="25" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1446,7 +1790,7 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
@@ -1463,7 +1807,7 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="24"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="13" t="s">
         <v>1</v>
       </c>
@@ -1485,20 +1829,20 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="27.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
     </row>
     <row r="16" spans="1:17" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2"/>
@@ -1514,7 +1858,7 @@
       <c r="G16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="24" t="s">
         <v>33</v>
       </c>
       <c r="I16" s="8" t="s">
@@ -1537,7 +1881,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1578,7 +1922,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="24"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
@@ -1617,7 +1961,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="24"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1655,8 +1999,313 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2">
+        <v>0.49176999999999998</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="25"/>
+      <c r="B26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2">
+        <v>0.47691</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="25"/>
+      <c r="B27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2">
+        <v>0.4899</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="25"/>
+      <c r="B33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="25"/>
+      <c r="B34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="25"/>
+      <c r="B40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="25"/>
+      <c r="B41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="11">
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A37:L37"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="G2:J2"/>

</xml_diff>

<commit_message>
add saving model function
</commit_message>
<xml_diff>
--- a/practicum-experiment.xlsx
+++ b/practicum-experiment.xlsx
@@ -606,10 +606,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -896,7 +896,7 @@
   <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -919,12 +919,12 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
@@ -1127,20 +1127,20 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
       <c r="M15" t="s">
         <v>40</v>
       </c>
@@ -1308,20 +1308,20 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2"/>
@@ -1410,20 +1410,20 @@
       <c r="L30" s="2"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2"/>
@@ -1464,7 +1464,9 @@
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="E35" s="2">
+        <v>0.37552000000000002</v>
+      </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -1480,7 +1482,9 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="E36" s="2">
+        <v>0.39889000000000002</v>
+      </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -1496,7 +1500,9 @@
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="E37" s="2">
+        <v>0.38457000000000002</v>
+      </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -1506,20 +1512,20 @@
       <c r="L37" s="2"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2"/>
@@ -1603,17 +1609,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A15:L15"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A33:L33"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A40:L40"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1624,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1647,12 +1653,12 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
@@ -1829,20 +1835,20 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="27.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
     </row>
     <row r="16" spans="1:17" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2"/>
@@ -2005,20 +2011,20 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2"/>
@@ -2107,20 +2113,20 @@
       <c r="L27" s="2"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2"/>
@@ -2161,7 +2167,9 @@
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="E32" s="2">
+        <v>0.47625000000000001</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -2177,7 +2185,9 @@
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="E33" s="2">
+        <v>0.47338999999999998</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -2193,7 +2203,9 @@
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="E34" s="2">
+        <v>0.48071999999999998</v>
+      </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2203,20 +2215,20 @@
       <c r="L34" s="2"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2"/>
@@ -2300,17 +2312,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A15:L15"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="A23:L23"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="A30:L30"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="A37:L37"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
change some parameter: batch_size = 64
</commit_message>
<xml_diff>
--- a/practicum-experiment.xlsx
+++ b/practicum-experiment.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="53">
   <si>
     <t>TD</t>
   </si>
@@ -483,7 +483,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -558,12 +558,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -610,6 +634,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -893,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S44"/>
+  <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1363,7 +1396,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2">
-        <v>0.36648999999999998</v>
+        <v>0.36739300000000003</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1381,7 +1414,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2">
-        <v>0.34767999999999999</v>
+        <v>0.348746</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -1399,7 +1432,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2">
-        <v>0.36029</v>
+        <v>0.36215999999999998</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1409,160 +1442,180 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2">
+        <v>0.37114999999999998</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="25"/>
+      <c r="B32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2">
+        <v>0.33685999999999999</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+    </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="25"/>
+      <c r="B33" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2">
+        <v>0.35493999999999998</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2">
-        <v>0.37552000000000002</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="25"/>
-      <c r="B36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2">
-        <v>0.39889000000000002</v>
-      </c>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="30"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="25"/>
-      <c r="B37" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="2">
-        <v>0.38457000000000002</v>
-      </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="25"/>
+      <c r="B39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="26"/>
-      <c r="K40" s="26"/>
-      <c r="L40" s="26"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
+      <c r="A41" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="25" t="s">
-        <v>17</v>
-      </c>
+      <c r="A42" s="25"/>
       <c r="B42" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1578,7 +1631,7 @@
     <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="25"/>
       <c r="B43" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1591,35 +1644,168 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="25"/>
-      <c r="B44" s="2" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+      <c r="L46" s="26"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="25"/>
+      <c r="B49" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="25"/>
+      <c r="B50" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="25"/>
+      <c r="B52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="25"/>
+      <c r="B53" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="14">
+    <mergeCell ref="A51:A53"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A15:L15"/>
-    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A48:A50"/>
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A33:L33"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A40:L40"/>
+    <mergeCell ref="A36:L36"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A46:L46"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A41:A43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1628,10 +1814,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:L30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48:E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2066,7 +2252,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2">
-        <v>0.49176999999999998</v>
+        <v>0.49141000000000001</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -2084,7 +2270,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2">
-        <v>0.47691</v>
+        <v>0.47817799999999999</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -2102,7 +2288,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2">
-        <v>0.4899</v>
+        <v>0.49160500000000001</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -2112,160 +2298,180 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2">
+        <v>0.49930999999999998</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="25"/>
+      <c r="B29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
+        <v>0.48335</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="25"/>
+      <c r="B30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2">
+        <v>0.48962</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2">
-        <v>0.47625000000000001</v>
-      </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="25"/>
-      <c r="B33" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2">
-        <v>0.47338999999999998</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="25"/>
-      <c r="B34" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="2">
-        <v>0.48071999999999998</v>
-      </c>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="25"/>
+      <c r="B36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="26"/>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26"/>
-      <c r="L37" s="26"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
+      <c r="A38" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="25" t="s">
-        <v>17</v>
-      </c>
+      <c r="A39" s="25"/>
       <c r="B39" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2281,7 +2487,7 @@
     <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="25"/>
       <c r="B40" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2294,35 +2500,168 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="25"/>
-      <c r="B41" s="2" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="26"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="25"/>
+      <c r="B46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="25"/>
+      <c r="B47" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="25"/>
+      <c r="B49" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="25"/>
+      <c r="B50" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="14">
+    <mergeCell ref="A48:A50"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A15:L15"/>
-    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A45:A47"/>
     <mergeCell ref="A23:L23"/>
     <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A30:L30"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A37:L37"/>
+    <mergeCell ref="A33:L33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A43:L43"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A38:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
generate 10 jumpmean dataset. Add random seed for reproducibility
</commit_message>
<xml_diff>
--- a/practicum-experiment.xlsx
+++ b/practicum-experiment.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="AUC" sheetId="1" r:id="rId1"/>
     <sheet name="F1" sheetId="2" r:id="rId2"/>
+    <sheet name="F1-Gen" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="97">
   <si>
     <t>TD</t>
   </si>
@@ -470,6 +471,134 @@
   </si>
   <si>
     <t xml:space="preserve">training: subject 1-&gt; 8 / validation: 9, 10 / testing: 11, 12. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>original code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> single 1D timeseries</t>
+    </r>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>TD: 3 channel, default param. FD: 1 channel</t>
+  </si>
+  <si>
+    <t>intermediate_dim_TD=16
+h=3, s = 2</t>
+  </si>
+  <si>
+    <t>TD 3 channel, intermediate 16, h= 3, s = 1</t>
+  </si>
+  <si>
+    <t>I = 8, h = 3, s = 1</t>
+  </si>
+  <si>
+    <t>intermediate = 8, h =2, s= 1</t>
+  </si>
+  <si>
+    <t>intermediate = 16, h = 2, s = 1</t>
+  </si>
+  <si>
+    <t>inter = 32, h = 3, s = 1</t>
+  </si>
+  <si>
+    <t>inter = 32, h = 4, s = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataset: 3 channels, 1 noise, two don't noise </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataset: 3 channels, 2 noise </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>original code:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> single 1D timeseries, channel 0</t>
+    </r>
+  </si>
+  <si>
+    <t>I = 8, h = 3, s = 2</t>
+  </si>
+  <si>
+    <t>##########################################################################################33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training score for 10 dataset. </t>
+  </si>
+  <si>
+    <t>Dataset 9</t>
+  </si>
+  <si>
+    <t>Dataset 10</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Purpose: check that TIRE doesn't vary in training but vary in testing</t>
+  </si>
+  <si>
+    <t>Alpha seetings</t>
+  </si>
+  <si>
+    <t>Only channel 0</t>
+  </si>
+  <si>
+    <t>Type dataset</t>
+  </si>
+  <si>
+    <t>Table 1: Tire on channel 0 only.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 2: TIRE on L2 norm </t>
+  </si>
+  <si>
+    <t>Table 3: Multi channel for TD: intermediate_dim 0, h_TD = 1, nr_shared_TD = 1</t>
+  </si>
+  <si>
+    <t>Table 4: Multi channel for TD: intermediate_dim 16, h_TD = 3, nr_shared_TD = 3</t>
   </si>
 </sst>
 </file>
@@ -528,7 +657,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -636,12 +765,220 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -685,6 +1022,21 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -699,10 +1051,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -714,6 +1066,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1021,12 +1444,12 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
@@ -1051,7 +1474,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -1083,7 +1506,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="25"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
@@ -1113,7 +1536,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="25"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
@@ -1146,7 +1569,7 @@
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="30" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1175,7 +1598,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="25"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
@@ -1202,7 +1625,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="25"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="13" t="s">
         <v>1</v>
       </c>
@@ -1229,20 +1652,20 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
       <c r="M15" t="s">
         <v>40</v>
       </c>
@@ -1281,7 +1704,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1322,7 +1745,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="25"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
@@ -1361,7 +1784,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="25"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1410,20 +1833,20 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2"/>
@@ -1456,7 +1879,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1490,7 +1913,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="25"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="2" t="s">
         <v>2</v>
       </c>
@@ -1522,7 +1945,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="25"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="2" t="s">
         <v>1</v>
       </c>
@@ -1554,7 +1977,7 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="30" t="s">
         <v>18</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1574,7 +1997,7 @@
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="25"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
@@ -1592,7 +2015,7 @@
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="25"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="2" t="s">
         <v>1</v>
       </c>
@@ -1610,20 +2033,20 @@
       <c r="L33" s="2"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
-      <c r="L36" s="30"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="34"/>
+      <c r="L36" s="35"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2"/>
@@ -1656,7 +2079,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1690,7 +2113,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="25"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1722,7 +2145,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="25"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="2" t="s">
         <v>1</v>
       </c>
@@ -1754,7 +2177,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="30" t="s">
         <v>18</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1772,7 +2195,7 @@
       <c r="L41" s="2"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="25"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="2" t="s">
         <v>2</v>
       </c>
@@ -1788,7 +2211,7 @@
       <c r="L42" s="2"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="25"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="2" t="s">
         <v>1</v>
       </c>
@@ -1804,20 +2227,20 @@
       <c r="L43" s="2"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="32"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2"/>
@@ -1850,7 +2273,7 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -1882,7 +2305,7 @@
       <c r="L48" s="2"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="25"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="2" t="s">
         <v>2</v>
       </c>
@@ -1912,7 +2335,7 @@
       <c r="L49" s="2"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="25"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="2" t="s">
         <v>1</v>
       </c>
@@ -1942,7 +2365,7 @@
       <c r="L50" s="2"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="25" t="s">
+      <c r="A51" s="30" t="s">
         <v>18</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -1976,7 +2399,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="25"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="2" t="s">
         <v>2</v>
       </c>
@@ -2008,7 +2431,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="25"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="2" t="s">
         <v>1</v>
       </c>
@@ -2065,8 +2488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2090,12 +2513,12 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
@@ -2120,7 +2543,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -2152,7 +2575,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="25"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
@@ -2182,7 +2605,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="25"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
@@ -2215,7 +2638,7 @@
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="30" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -2233,7 +2656,7 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="25"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
@@ -2250,7 +2673,7 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="25"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="13" t="s">
         <v>1</v>
       </c>
@@ -2272,20 +2695,20 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="27.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
     </row>
     <row r="16" spans="1:17" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2"/>
@@ -2324,7 +2747,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2365,7 +2788,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="25"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
@@ -2404,7 +2827,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="25"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
@@ -2448,20 +2871,20 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2"/>
@@ -2500,7 +2923,7 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2542,7 +2965,7 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="25"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
@@ -2582,7 +3005,7 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="25"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="2" t="s">
         <v>1</v>
       </c>
@@ -2622,7 +3045,7 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="30" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2642,7 +3065,7 @@
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="25"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="2" t="s">
         <v>2</v>
       </c>
@@ -2660,7 +3083,7 @@
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="25"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="2" t="s">
         <v>1</v>
       </c>
@@ -2678,27 +3101,27 @@
       <c r="L30" s="2"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="32" t="s">
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="N33" s="31" t="s">
+      <c r="N33" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="O33" s="33" t="s">
+      <c r="O33" s="38" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2731,12 +3154,12 @@
       <c r="L34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M34" s="32"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="33"/>
+      <c r="M34" s="36"/>
+      <c r="N34" s="37"/>
+      <c r="O34" s="38"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2784,7 +3207,7 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="25"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -2830,7 +3253,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="25"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="2" t="s">
         <v>1</v>
       </c>
@@ -2876,7 +3299,7 @@
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="30" t="s">
         <v>18</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2894,7 +3317,7 @@
       <c r="L38" s="2"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="25"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
@@ -2910,7 +3333,7 @@
       <c r="L39" s="2"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="25"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="2" t="s">
         <v>1</v>
       </c>
@@ -2926,27 +3349,27 @@
       <c r="L40" s="2"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="34" t="s">
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="32"/>
+      <c r="M43" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="N43" s="35" t="s">
+      <c r="N43" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="O43" s="33" t="s">
+      <c r="O43" s="38" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2979,12 +3402,12 @@
       <c r="L44" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M44" s="34"/>
-      <c r="N44" s="35"/>
-      <c r="O44" s="33"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="40"/>
+      <c r="O44" s="38"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -3032,7 +3455,7 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="25"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="2" t="s">
         <v>2</v>
       </c>
@@ -3078,7 +3501,7 @@
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="25"/>
+      <c r="A47" s="30"/>
       <c r="B47" s="2" t="s">
         <v>1</v>
       </c>
@@ -3124,7 +3547,7 @@
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="30" t="s">
         <v>18</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -3158,7 +3581,7 @@
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="25"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="2" t="s">
         <v>2</v>
       </c>
@@ -3190,7 +3613,7 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="25"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="2" t="s">
         <v>1</v>
       </c>
@@ -3247,4 +3670,1328 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:O52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:M43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.89453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.78873239436619702</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.58695652173913004</v>
+      </c>
+      <c r="E4">
+        <v>0.52777777777000001</v>
+      </c>
+      <c r="F4">
+        <v>0.54736842105263095</v>
+      </c>
+      <c r="G4">
+        <v>0.512820512820512</v>
+      </c>
+      <c r="H4">
+        <v>0.48214285714285698</v>
+      </c>
+      <c r="I4">
+        <v>0.51685393258426904</v>
+      </c>
+      <c r="J4">
+        <v>0.531645569620253</v>
+      </c>
+      <c r="K4" s="17">
+        <v>0.59740259740259705</v>
+      </c>
+      <c r="L4">
+        <v>0.48598130841121401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="30"/>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.83783783783783705</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.58333333333333004</v>
+      </c>
+      <c r="E5">
+        <v>0.58333333333299997</v>
+      </c>
+      <c r="F5">
+        <v>0.58333333330000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="30"/>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.84210526315789402</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.60215053763439996</v>
+      </c>
+      <c r="E6">
+        <v>0.57142857142000003</v>
+      </c>
+      <c r="F6">
+        <v>0.56338028159999998</v>
+      </c>
+      <c r="G6">
+        <v>0.54736842105263095</v>
+      </c>
+      <c r="H6">
+        <v>0.56310679611650405</v>
+      </c>
+      <c r="I6">
+        <v>0.57425742574257399</v>
+      </c>
+      <c r="J6">
+        <v>0.53465346534653402</v>
+      </c>
+      <c r="K6">
+        <v>0.60194174757281504</v>
+      </c>
+      <c r="L6">
+        <v>0.60869565217391297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="L10" s="29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0.84705882352941098</v>
+      </c>
+      <c r="D11">
+        <v>0.60344827586206895</v>
+      </c>
+      <c r="E11">
+        <v>0.3809523809</v>
+      </c>
+      <c r="F11">
+        <v>0.35862068899999999</v>
+      </c>
+      <c r="G11">
+        <v>0.79999900000000002</v>
+      </c>
+      <c r="H11">
+        <v>0.79999900000000002</v>
+      </c>
+      <c r="I11">
+        <v>0.325581395</v>
+      </c>
+      <c r="K11">
+        <v>0.40277777770000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="30"/>
+      <c r="B12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>0.86666600000000005</v>
+      </c>
+      <c r="D12">
+        <v>0.60176991150442405</v>
+      </c>
+      <c r="H12">
+        <v>0.601769</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="30"/>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0.87640399999999996</v>
+      </c>
+      <c r="D13">
+        <v>0.6</v>
+      </c>
+      <c r="E13">
+        <v>0.55813900000000005</v>
+      </c>
+      <c r="F13">
+        <v>0.56603769999999998</v>
+      </c>
+      <c r="G13">
+        <v>0.64220100000000002</v>
+      </c>
+      <c r="H13">
+        <v>0.72548999999999997</v>
+      </c>
+      <c r="I13">
+        <v>0.55445540000000004</v>
+      </c>
+      <c r="K13">
+        <v>0.49612400000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="L19" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="M19" s="44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.86315789473684201</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.86666600000000005</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.93333333330000001</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.82105262999999995</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.87640449399999998</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.83146067415000002</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.88421052600000005</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.85393258425999996</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0.92307692299999999</v>
+      </c>
+      <c r="M20" s="46">
+        <v>0.82352941099999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="47"/>
+      <c r="B21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="31"/>
+      <c r="D21" s="2">
+        <v>0.84536082474226804</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.85714279999999998</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.89655172400000005</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.82758620000000005</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.83146067400000001</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.79069767400000002</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.90109890100000001</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0.869565217</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0.89361702119999997</v>
+      </c>
+      <c r="M21" s="46">
+        <v>0.82352941099999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="47"/>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="31"/>
+      <c r="D22" s="2">
+        <v>0.85416666600000002</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.88372092999999996</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.89361699999999999</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.84444443999999996</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.85057471200000001</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.82978722999999999</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.90109890100000001</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0.88888880000000003</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0.88172043</v>
+      </c>
+      <c r="M22" s="46">
+        <v>0.83720930000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="47"/>
+      <c r="B23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.85714285714000005</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.88372092999999996</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.91489361700000005</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.78048780399999995</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.87912087910000003</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.88172043</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.89583299999999999</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0.80898876399999997</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.87999998999999995</v>
+      </c>
+      <c r="M23" s="46">
+        <v>0.86315789399999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="47"/>
+      <c r="B24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="31"/>
+      <c r="D24" s="2">
+        <v>0.83870967699999999</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.90526315000000002</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.88421052</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.79012345678999996</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.87640448999999998</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.86666600000000005</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.88172043</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.83333332999999998</v>
+      </c>
+      <c r="M24" s="46">
+        <v>0.85714285710000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A25" s="48"/>
+      <c r="B25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="49"/>
+      <c r="D25" s="6">
+        <v>0.84444439999999998</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.90322579999999997</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.91489361000000002</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0.808988764044</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0.87912087910000003</v>
+      </c>
+      <c r="I25" s="6">
+        <v>0.87640448999999998</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0.89130434000000003</v>
+      </c>
+      <c r="K25" s="6">
+        <v>0.82222222</v>
+      </c>
+      <c r="L25" s="6">
+        <v>0.88421050000000001</v>
+      </c>
+      <c r="M25" s="50">
+        <v>0.86666666660000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A26" s="54"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="62" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="64"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="65"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L28" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="M28" s="46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.85714285714000005</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.88372092999999996</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.91489361700000005</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.78048780399999995</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.87912087910000003</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.88172043</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.89583299999999999</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0.80898876399999997</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0.87999998999999995</v>
+      </c>
+      <c r="M29" s="46">
+        <v>0.86315789399999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="60"/>
+      <c r="B30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="31"/>
+      <c r="D30" s="2">
+        <v>0.83870967699999999</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.90526315000000002</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.88421052</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.79012345678999996</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.87640448999999998</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0.86666600000000005</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0.88172043</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0.83333332999999998</v>
+      </c>
+      <c r="M30" s="46">
+        <v>0.85714285710000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A31" s="61"/>
+      <c r="B31" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="49"/>
+      <c r="D31" s="6">
+        <v>0.84444439999999998</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0.90322579999999997</v>
+      </c>
+      <c r="F31" s="6">
+        <v>0.91489361000000002</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0.808988764044</v>
+      </c>
+      <c r="H31" s="6">
+        <v>0.87912087910000003</v>
+      </c>
+      <c r="I31" s="6">
+        <v>0.87640448999999998</v>
+      </c>
+      <c r="J31" s="6">
+        <v>0.89130434000000003</v>
+      </c>
+      <c r="K31" s="6">
+        <v>0.82222222</v>
+      </c>
+      <c r="L31" s="6">
+        <v>0.88421050000000001</v>
+      </c>
+      <c r="M31" s="50">
+        <v>0.86666666660000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="56"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A33" s="53"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="58"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="59"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J35" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L35" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="M35" s="46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="60"/>
+      <c r="B36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0.69662921</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.68041237099999996</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.65957446799999997</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.58490565999999999</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0.59770113999999996</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0.67415729999999996</v>
+      </c>
+      <c r="K36" s="2">
+        <v>0.58947360000000004</v>
+      </c>
+      <c r="L36" s="2">
+        <v>0.65384615300000004</v>
+      </c>
+      <c r="M36" s="46">
+        <v>0.71910112000000004</v>
+      </c>
+      <c r="N36">
+        <f>AVERAGE(D36:M36)</f>
+        <v>0.64558010219999995</v>
+      </c>
+      <c r="O36">
+        <f>_xlfn.STDEV.S(D36:M36)</f>
+        <v>4.8881640251010994E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="60"/>
+      <c r="B37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="31"/>
+      <c r="D37" s="2">
+        <v>0.58394160579999999</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.67469878999999999</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.66666665999999997</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0.60176991000000002</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0.59090909000000003</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0.7111111</v>
+      </c>
+      <c r="K37" s="2">
+        <v>0.55445544000000002</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0.70103092779999998</v>
+      </c>
+      <c r="M37" s="46">
+        <v>0.77419354799999995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="45"/>
+      <c r="B38" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="67"/>
+      <c r="D38" s="66">
+        <v>0.59420289000000004</v>
+      </c>
+      <c r="E38" s="66">
+        <v>0.67272726999999999</v>
+      </c>
+      <c r="F38" s="66">
+        <v>0.67368419999999996</v>
+      </c>
+      <c r="G38" s="66">
+        <v>0.67368421052600003</v>
+      </c>
+      <c r="H38" s="66">
+        <v>0.60674156999999995</v>
+      </c>
+      <c r="I38" s="66">
+        <v>0.6086956</v>
+      </c>
+      <c r="J38" s="66">
+        <v>0.69473684000000002</v>
+      </c>
+      <c r="K38" s="66">
+        <v>0.5625</v>
+      </c>
+      <c r="L38" s="66">
+        <v>0.68686868000000001</v>
+      </c>
+      <c r="M38" s="68">
+        <v>0.72340424999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="69"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A40" s="69"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="58"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="58"/>
+      <c r="J41" s="58"/>
+      <c r="K41" s="58"/>
+      <c r="L41" s="58"/>
+      <c r="M41" s="59"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="65"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H42" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J42" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L42" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="M42" s="46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.84705882349999995</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0.76470587999999995</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.7916666</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0.784810126</v>
+      </c>
+      <c r="H43" s="18">
+        <v>0.41025641000000002</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0.72340424999999997</v>
+      </c>
+      <c r="J43" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="K43" s="2">
+        <v>0.76767669999999999</v>
+      </c>
+      <c r="L43" s="2">
+        <v>0.80459770113999995</v>
+      </c>
+      <c r="M43" s="51">
+        <v>0.68</v>
+      </c>
+      <c r="N43">
+        <f>AVERAGE(D43:M43)</f>
+        <v>0.73241764906399998</v>
+      </c>
+      <c r="O43">
+        <f>_xlfn.STDEV.S(D43:M43)</f>
+        <v>0.12193785004661728</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="60"/>
+      <c r="B44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="31"/>
+      <c r="D44" s="2">
+        <v>0.58394160579999999</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0.67469879509999997</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.66666665999999997</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="H44" s="52">
+        <v>0.60176991150000003</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0.59090900000000002</v>
+      </c>
+      <c r="J44" s="2">
+        <v>0.71111111100000002</v>
+      </c>
+      <c r="K44" s="2">
+        <v>0.55445500000000003</v>
+      </c>
+      <c r="L44" s="2">
+        <v>0.70103092782999998</v>
+      </c>
+      <c r="M44" s="46">
+        <v>0.77419354838700005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A45" s="61"/>
+      <c r="B45" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="49"/>
+      <c r="D45" s="6">
+        <v>0.66666666600000002</v>
+      </c>
+      <c r="E45" s="6">
+        <v>0.77647058000000002</v>
+      </c>
+      <c r="F45" s="6">
+        <v>0.75268817200000004</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0.79999989999999999</v>
+      </c>
+      <c r="H45" s="71">
+        <v>0.57999990000000001</v>
+      </c>
+      <c r="I45" s="6">
+        <v>0.64367816</v>
+      </c>
+      <c r="J45" s="6">
+        <v>0.77777770000000002</v>
+      </c>
+      <c r="K45" s="6">
+        <v>0.61682242899999995</v>
+      </c>
+      <c r="L45" s="6">
+        <v>0.73333333329999995</v>
+      </c>
+      <c r="M45" s="50">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="31"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H49" s="70" t="s">
+        <v>46</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J49" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L49" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.50331125827000001</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0.40287769784100003</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.43548387096699998</v>
+      </c>
+      <c r="G50" s="2">
+        <v>0.52777777699999995</v>
+      </c>
+      <c r="H50" s="18">
+        <v>0.735632183</v>
+      </c>
+      <c r="I50" s="2">
+        <v>0.46896550999999997</v>
+      </c>
+      <c r="J50" s="2">
+        <v>0.42105263100000001</v>
+      </c>
+      <c r="K50" s="18">
+        <v>0.625</v>
+      </c>
+      <c r="L50" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="M50" s="52">
+        <v>0.45255474452</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="30"/>
+      <c r="B51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="31"/>
+      <c r="D51" s="2">
+        <v>0.58394159999999995</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0.67469879517999998</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.66666665999999997</v>
+      </c>
+      <c r="G51" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="H51" s="52">
+        <v>0.60176991150000003</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0.59090900000000002</v>
+      </c>
+      <c r="J51" s="2">
+        <v>0.71111111100000002</v>
+      </c>
+      <c r="K51" s="2">
+        <v>0.55445500000000003</v>
+      </c>
+      <c r="L51" s="2">
+        <v>0.70103092782999998</v>
+      </c>
+      <c r="M51" s="2">
+        <v>0.77419354838700005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="30"/>
+      <c r="B52" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="31"/>
+      <c r="D52" s="2">
+        <v>0.53608247421999999</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0.65979381439999996</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.61224489790000003</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0.64444444440000004</v>
+      </c>
+      <c r="H52" s="52">
+        <v>0.65979381000000004</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0.55319147999999996</v>
+      </c>
+      <c r="J52" s="2">
+        <v>0.59090909000000003</v>
+      </c>
+      <c r="K52" s="2">
+        <v>0.55445544550000003</v>
+      </c>
+      <c r="L52" s="2">
+        <v>0.70833333330000003</v>
+      </c>
+      <c r="M52" s="2">
+        <v>0.60952380900000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="A34:M34"/>
+    <mergeCell ref="A41:M41"/>
+    <mergeCell ref="A48:M48"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="A20:A25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
seperate test experiment into 3 files, change save path for metrics
</commit_message>
<xml_diff>
--- a/practicum-experiment.xlsx
+++ b/practicum-experiment.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AUC" sheetId="1" r:id="rId1"/>
-    <sheet name="F1" sheetId="2" r:id="rId2"/>
-    <sheet name="F1-Gen" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="F1" sheetId="2" r:id="rId3"/>
+    <sheet name="F1-jumpmean_ar" sheetId="3" r:id="rId4"/>
+    <sheet name="F1-jumpmean-gauss" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="100">
   <si>
     <t>TD</t>
   </si>
@@ -443,9 +445,6 @@
     <t>Std</t>
   </si>
   <si>
-    <t>pvalue=0.83</t>
-  </si>
-  <si>
     <t>Not significant</t>
   </si>
   <si>
@@ -458,13 +457,7 @@
     <t>pair t-test with original</t>
   </si>
   <si>
-    <t>pvalue=0.9578</t>
-  </si>
-  <si>
     <t>pvalue=0.9174</t>
-  </si>
-  <si>
-    <t>pvalue=0.9795</t>
   </si>
   <si>
     <t>pvalue=0.9205</t>
@@ -606,12 +599,24 @@
   <si>
     <t>Table 6: DMD</t>
   </si>
+  <si>
+    <t>Method 2: ICA -&gt; L2 norm, instance 1</t>
+  </si>
+  <si>
+    <t>Method 3: ICA -&gt; DMD norm, instance 2</t>
+  </si>
+  <si>
+    <t>t-Test: Two-Sample Assuming Equal Variances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 1: TIRE on channel 0 </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,6 +654,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -663,7 +676,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -979,12 +992,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1080,6 +1126,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1145,6 +1202,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1453,12 +1525,12 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:19" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
@@ -1483,7 +1555,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -1515,7 +1587,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="49"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
@@ -1545,7 +1617,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="49"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
@@ -1578,7 +1650,7 @@
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="54" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1607,7 +1679,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="49"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
@@ -1634,7 +1706,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="49"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="13" t="s">
         <v>1</v>
       </c>
@@ -1661,20 +1733,20 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
       <c r="M15" t="s">
         <v>40</v>
       </c>
@@ -1713,7 +1785,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1754,7 +1826,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="49"/>
+      <c r="A18" s="54"/>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
@@ -1793,7 +1865,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="49"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1842,20 +1914,20 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="51" t="s">
+      <c r="A26" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
+      <c r="J26" s="56"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2"/>
@@ -1888,7 +1960,7 @@
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1922,7 +1994,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="49"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="2" t="s">
         <v>2</v>
       </c>
@@ -1954,7 +2026,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="49"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="2" t="s">
         <v>1</v>
       </c>
@@ -1986,7 +2058,7 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="54" t="s">
         <v>18</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -2006,7 +2078,7 @@
       <c r="L31" s="2"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="49"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
@@ -2024,7 +2096,7 @@
       <c r="L32" s="2"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="49"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="2" t="s">
         <v>1</v>
       </c>
@@ -2042,20 +2114,20 @@
       <c r="L33" s="2"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="53"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="53"/>
-      <c r="L36" s="54"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="58"/>
+      <c r="K36" s="58"/>
+      <c r="L36" s="59"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2"/>
@@ -2088,7 +2160,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="49" t="s">
+      <c r="A38" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2122,7 +2194,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="49"/>
+      <c r="A39" s="54"/>
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
@@ -2154,7 +2226,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="49"/>
+      <c r="A40" s="54"/>
       <c r="B40" s="2" t="s">
         <v>1</v>
       </c>
@@ -2186,7 +2258,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="54" t="s">
         <v>18</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -2204,7 +2276,7 @@
       <c r="L41" s="2"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="49"/>
+      <c r="A42" s="54"/>
       <c r="B42" s="2" t="s">
         <v>2</v>
       </c>
@@ -2220,7 +2292,7 @@
       <c r="L42" s="2"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="49"/>
+      <c r="A43" s="54"/>
       <c r="B43" s="2" t="s">
         <v>1</v>
       </c>
@@ -2236,20 +2308,20 @@
       <c r="L43" s="2"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="51" t="s">
+      <c r="A46" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
-      <c r="I46" s="51"/>
-      <c r="J46" s="51"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="51"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="56"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="56"/>
+      <c r="L46" s="56"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2"/>
@@ -2282,7 +2354,7 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="49" t="s">
+      <c r="A48" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -2314,7 +2386,7 @@
       <c r="L48" s="2"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="49"/>
+      <c r="A49" s="54"/>
       <c r="B49" s="2" t="s">
         <v>2</v>
       </c>
@@ -2344,7 +2416,7 @@
       <c r="L49" s="2"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="49"/>
+      <c r="A50" s="54"/>
       <c r="B50" s="2" t="s">
         <v>1</v>
       </c>
@@ -2374,7 +2446,7 @@
       <c r="L50" s="2"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="49" t="s">
+      <c r="A51" s="54" t="s">
         <v>18</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -2408,7 +2480,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="49"/>
+      <c r="A52" s="54"/>
       <c r="B52" s="2" t="s">
         <v>2</v>
       </c>
@@ -2440,7 +2512,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="49"/>
+      <c r="A53" s="54"/>
       <c r="B53" s="2" t="s">
         <v>1</v>
       </c>
@@ -2495,10 +2567,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q50"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="B21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="36.83984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T70"/>
+  <sheetViews>
+    <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2514,6 +2610,7 @@
     <col min="13" max="13" width="12.734375" customWidth="1"/>
     <col min="15" max="15" width="12.20703125" customWidth="1"/>
     <col min="16" max="16" width="11.9453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -2522,12 +2619,12 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:17" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11"/>
@@ -2552,7 +2649,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -2584,7 +2681,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="49"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
@@ -2614,7 +2711,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="49"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
@@ -2647,7 +2744,7 @@
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="54" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -2665,7 +2762,7 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="49"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="12" t="s">
         <v>2</v>
       </c>
@@ -2682,7 +2779,7 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="49"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="13" t="s">
         <v>1</v>
       </c>
@@ -2704,20 +2801,20 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="27.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="55"/>
     </row>
     <row r="16" spans="1:17" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2"/>
@@ -2756,7 +2853,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="49" t="s">
+      <c r="A17" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2797,7 +2894,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="49"/>
+      <c r="A18" s="54"/>
       <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
@@ -2836,7 +2933,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="49"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
@@ -2876,24 +2973,24 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="E22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2"/>
@@ -2932,7 +3029,7 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2974,7 +3071,7 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="49"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
@@ -3014,7 +3111,7 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="49"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="2" t="s">
         <v>1</v>
       </c>
@@ -3054,7 +3151,7 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="54" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -3074,7 +3171,7 @@
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="49"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="2" t="s">
         <v>2</v>
       </c>
@@ -3092,7 +3189,7 @@
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="49"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="2" t="s">
         <v>1</v>
       </c>
@@ -3109,32 +3206,32 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="51" t="s">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="51"/>
-      <c r="M33" s="55" t="s">
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="N33" s="56" t="s">
+      <c r="N33" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="O33" s="57" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O33" s="62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3163,12 +3260,12 @@
       <c r="L34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M34" s="55"/>
-      <c r="N34" s="56"/>
-      <c r="O34" s="57"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="49" t="s">
+      <c r="M34" s="60"/>
+      <c r="N34" s="61"/>
+      <c r="O34" s="62"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -3208,15 +3305,18 @@
         <f>_xlfn.STDEV.S(E35:L35)</f>
         <v>8.507376890713754E-2</v>
       </c>
-      <c r="O35" t="s">
+      <c r="O35">
+        <v>0.95592521799999997</v>
+      </c>
+      <c r="P35" t="s">
         <v>58</v>
       </c>
-      <c r="P35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="49"/>
+      <c r="R35" s="53"/>
+      <c r="S35" s="53"/>
+      <c r="T35" s="53"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="54"/>
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -3254,15 +3354,15 @@
         <f t="shared" ref="N36:N37" si="4">_xlfn.STDEV.S(E36:L36)</f>
         <v>8.5670458347076206E-2</v>
       </c>
-      <c r="O36" t="s">
-        <v>63</v>
-      </c>
       <c r="P36" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="49"/>
+        <v>58</v>
+      </c>
+      <c r="R36" s="51"/>
+      <c r="S36" s="51"/>
+      <c r="T36" s="51"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="54"/>
       <c r="B37" s="2" t="s">
         <v>1</v>
       </c>
@@ -3300,15 +3400,15 @@
         <f t="shared" si="4"/>
         <v>8.5151272357265315E-2</v>
       </c>
-      <c r="O37" t="s">
-        <v>65</v>
-      </c>
       <c r="P37" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="R37" s="51"/>
+      <c r="S37" s="51"/>
+      <c r="T37" s="51"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="54" t="s">
         <v>18</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -3324,9 +3424,12 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="49"/>
+      <c r="R38" s="51"/>
+      <c r="S38" s="51"/>
+      <c r="T38" s="51"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="54"/>
       <c r="B39" s="2" t="s">
         <v>2</v>
       </c>
@@ -3340,9 +3443,12 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="49"/>
+      <c r="R39" s="51"/>
+      <c r="S39" s="51"/>
+      <c r="T39" s="51"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="54"/>
       <c r="B40" s="2" t="s">
         <v>1</v>
       </c>
@@ -3356,33 +3462,49 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="51" t="s">
+      <c r="R40" s="51"/>
+      <c r="S40" s="51"/>
+      <c r="T40" s="51"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="R41" s="51"/>
+      <c r="S41" s="51"/>
+      <c r="T41" s="51"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="R42" s="51"/>
+      <c r="S42" s="51"/>
+      <c r="T42" s="51"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="51"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
-      <c r="F43" s="51"/>
-      <c r="G43" s="51"/>
-      <c r="H43" s="51"/>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
-      <c r="K43" s="51"/>
-      <c r="L43" s="51"/>
-      <c r="M43" s="58" t="s">
+      <c r="B43" s="56"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="56"/>
+      <c r="E43" s="56"/>
+      <c r="F43" s="56"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="56"/>
+      <c r="I43" s="56"/>
+      <c r="J43" s="56"/>
+      <c r="K43" s="56"/>
+      <c r="L43" s="56"/>
+      <c r="M43" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="N43" s="59" t="s">
+      <c r="N43" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="O43" s="57" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O43" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="R43" s="51"/>
+      <c r="S43" s="51"/>
+      <c r="T43" s="51"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3411,12 +3533,15 @@
       <c r="L44" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M44" s="58"/>
-      <c r="N44" s="59"/>
-      <c r="O44" s="57"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="49" t="s">
+      <c r="M44" s="63"/>
+      <c r="N44" s="64"/>
+      <c r="O44" s="62"/>
+      <c r="R44" s="51"/>
+      <c r="S44" s="51"/>
+      <c r="T44" s="51"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -3457,14 +3582,17 @@
         <v>7.809626266384509E-2</v>
       </c>
       <c r="O45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P45" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="49"/>
+        <v>58</v>
+      </c>
+      <c r="R45" s="51"/>
+      <c r="S45" s="51"/>
+      <c r="T45" s="51"/>
+    </row>
+    <row r="46" spans="1:20" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A46" s="54"/>
       <c r="B46" s="2" t="s">
         <v>2</v>
       </c>
@@ -3503,14 +3631,17 @@
         <v>7.9737158817947684E-2</v>
       </c>
       <c r="O46" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P46" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="49"/>
+        <v>58</v>
+      </c>
+      <c r="R46" s="52"/>
+      <c r="S46" s="52"/>
+      <c r="T46" s="52"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="54"/>
       <c r="B47" s="2" t="s">
         <v>1</v>
       </c>
@@ -3549,14 +3680,14 @@
         <v>7.6547759557432565E-2</v>
       </c>
       <c r="O47" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P47" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="54" t="s">
         <v>18</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -3589,8 +3720,8 @@
         <v>0.57327935222672</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="49"/>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="54"/>
       <c r="B49" s="2" t="s">
         <v>2</v>
       </c>
@@ -3621,8 +3752,8 @@
         <v>0.576766856214459</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="49"/>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="54"/>
       <c r="B50" s="2" t="s">
         <v>1</v>
       </c>
@@ -3653,8 +3784,450 @@
         <v>0.57860615883306299</v>
       </c>
     </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="56"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="56"/>
+      <c r="H53" s="56"/>
+      <c r="I53" s="56"/>
+      <c r="J53" s="56"/>
+      <c r="K53" s="56"/>
+      <c r="L53" s="56"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M54" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N54" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2">
+        <v>0.46978193146399999</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0.46181818181000001</v>
+      </c>
+      <c r="G55" s="2">
+        <v>0.38835978835899998</v>
+      </c>
+      <c r="H55" s="2">
+        <v>0.57863304577999997</v>
+      </c>
+      <c r="I55" s="2">
+        <v>0.39225806451</v>
+      </c>
+      <c r="J55" s="2">
+        <v>0.37664567830559997</v>
+      </c>
+      <c r="K55" s="2">
+        <v>0.57393850658000001</v>
+      </c>
+      <c r="L55" s="2">
+        <v>0.55563331000600003</v>
+      </c>
+      <c r="M55">
+        <f>AVERAGE(E55:L55)</f>
+        <v>0.47463356335182494</v>
+      </c>
+      <c r="N55">
+        <f>_xlfn.STDEV.S(E55:L55)</f>
+        <v>8.5570862919689419E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="54"/>
+      <c r="B56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2">
+        <v>0.44430919050500001</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.45431789737</v>
+      </c>
+      <c r="G56" s="2">
+        <v>0.37568455640743997</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0.57666214382600001</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0.38556701030899998</v>
+      </c>
+      <c r="J56" s="2">
+        <v>0.38055720213389999</v>
+      </c>
+      <c r="K56" s="2">
+        <v>0.55733148019400003</v>
+      </c>
+      <c r="L56" s="2">
+        <v>0.57344632768299997</v>
+      </c>
+      <c r="M56">
+        <f t="shared" ref="M56:M60" si="7">AVERAGE(E56:L56)</f>
+        <v>0.46848447605354249</v>
+      </c>
+      <c r="N56">
+        <f t="shared" ref="N56:N60" si="8">_xlfn.STDEV.S(E56:L56)</f>
+        <v>8.8331082816394998E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="54"/>
+      <c r="B57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2">
+        <v>0.46586345381499999</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.46192573945799997</v>
+      </c>
+      <c r="G57" s="2">
+        <v>0.38021638330750002</v>
+      </c>
+      <c r="H57" s="2">
+        <v>0.58192505510000003</v>
+      </c>
+      <c r="I57" s="2">
+        <v>0.39577464788</v>
+      </c>
+      <c r="J57" s="2">
+        <v>0.38430926661999998</v>
+      </c>
+      <c r="K57" s="2">
+        <v>0.57656200000000002</v>
+      </c>
+      <c r="L57" s="2">
+        <v>0.565157750342</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="7"/>
+        <v>0.47646678706531254</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="8"/>
+        <v>8.7504145030205038E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2">
+        <v>0.4625935162</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0.46997389032999998</v>
+      </c>
+      <c r="G58" s="2">
+        <v>0.38373983739</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0.57606177606099995</v>
+      </c>
+      <c r="I58" s="2">
+        <v>0.39624005784499999</v>
+      </c>
+      <c r="J58" s="2">
+        <v>0.40298507462599997</v>
+      </c>
+      <c r="K58" s="2">
+        <v>0.57056145670000002</v>
+      </c>
+      <c r="L58" s="2">
+        <v>0.55982274740000004</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="7"/>
+        <v>0.477747294569</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="8"/>
+        <v>8.1395743928136199E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="54"/>
+      <c r="B59" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2">
+        <v>0.43893129770900002</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0.45768772348030001</v>
+      </c>
+      <c r="G59" s="2">
+        <v>0.378657487091</v>
+      </c>
+      <c r="H59" s="2">
+        <v>0.576798444588</v>
+      </c>
+      <c r="I59" s="2">
+        <v>0.37591973244139998</v>
+      </c>
+      <c r="J59" s="2">
+        <v>0.37520215633420001</v>
+      </c>
+      <c r="K59" s="2">
+        <v>0.56187290969000003</v>
+      </c>
+      <c r="L59" s="2">
+        <v>0.57317903329999997</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="7"/>
+        <v>0.46728109807923746</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="8"/>
+        <v>9.0814844428545621E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="54"/>
+      <c r="B60" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2">
+        <v>0.45960264899999997</v>
+      </c>
+      <c r="F60" s="2">
+        <v>0.46859296482399998</v>
+      </c>
+      <c r="G60" s="2">
+        <v>0.380085653104</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0.57256145915000001</v>
+      </c>
+      <c r="I60" s="2">
+        <v>0.389391979301</v>
+      </c>
+      <c r="J60" s="2">
+        <v>0.38910947249</v>
+      </c>
+      <c r="K60" s="2">
+        <v>0.57642585550000003</v>
+      </c>
+      <c r="L60" s="2">
+        <v>0.56970509380000001</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="7"/>
+        <v>0.47568439089612502</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="8"/>
+        <v>8.6819622393677978E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" s="56"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="56"/>
+      <c r="G63" s="56"/>
+      <c r="H63" s="56"/>
+      <c r="I63" s="56"/>
+      <c r="J63" s="56"/>
+      <c r="K63" s="56"/>
+      <c r="L63" s="56"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J64" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="54"/>
+      <c r="B66" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="54"/>
+      <c r="B67" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="54"/>
+      <c r="B69" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="54"/>
+      <c r="B70" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="26">
     <mergeCell ref="M33:M34"/>
     <mergeCell ref="N33:N34"/>
     <mergeCell ref="O33:O34"/>
@@ -3675,18 +4248,24 @@
     <mergeCell ref="A43:L43"/>
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="A53:L53"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A63:L63"/>
+    <mergeCell ref="A65:A67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3697,45 +4276,45 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="E2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="27" t="s">
+      <c r="H3" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="I3" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="29" t="s">
+      <c r="K3" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="I3" s="29" t="s">
+      <c r="L3" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="J3" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="L3" s="29" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3773,7 +4352,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="49"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
@@ -3791,7 +4370,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="49"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
@@ -3828,45 +4407,45 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="E9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="28" t="s">
+      <c r="G10" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="I10" s="29" t="s">
+      <c r="K10" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="K10" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="L10" s="29" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="54" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3898,7 +4477,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="49"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
@@ -3913,7 +4492,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="49"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
@@ -3944,27 +4523,27 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="31"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D19" s="33" t="s">
         <v>42</v>
@@ -3991,21 +4570,21 @@
         <v>49</v>
       </c>
       <c r="L19" s="33" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M19" s="34" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="66" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="50" t="s">
-        <v>87</v>
+      <c r="C20" s="55" t="s">
+        <v>84</v>
       </c>
       <c r="D20" s="2">
         <v>0.86315789473684201</v>
@@ -4039,11 +4618,11 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="62"/>
+      <c r="A21" s="67"/>
       <c r="B21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="50"/>
+      <c r="C21" s="55"/>
       <c r="D21" s="2">
         <v>0.84536082474226804</v>
       </c>
@@ -4076,11 +4655,11 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="62"/>
+      <c r="A22" s="67"/>
       <c r="B22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="50"/>
+      <c r="C22" s="55"/>
       <c r="D22" s="2">
         <v>0.85416666600000002</v>
       </c>
@@ -4113,12 +4692,12 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="62"/>
+      <c r="A23" s="67"/>
       <c r="B23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="50" t="s">
-        <v>88</v>
+      <c r="C23" s="55" t="s">
+        <v>85</v>
       </c>
       <c r="D23" s="2">
         <v>0.85714285714000005</v>
@@ -4152,11 +4731,11 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="62"/>
+      <c r="A24" s="67"/>
       <c r="B24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="50"/>
+      <c r="C24" s="55"/>
       <c r="D24" s="2">
         <v>0.83870967699999999</v>
       </c>
@@ -4189,11 +4768,11 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A25" s="63"/>
+      <c r="A25" s="68"/>
       <c r="B25" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="60"/>
+      <c r="C25" s="65"/>
       <c r="D25" s="6">
         <v>0.84444439999999998</v>
       </c>
@@ -4241,27 +4820,27 @@
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="67" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
-      <c r="M27" s="69"/>
+      <c r="A27" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="73"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73"/>
+      <c r="I27" s="73"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="73"/>
+      <c r="M27" s="74"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="43"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D28" s="26" t="s">
         <v>42</v>
@@ -4288,21 +4867,21 @@
         <v>49</v>
       </c>
       <c r="L28" s="26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M28" s="35" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="64" t="s">
+      <c r="A29" s="69" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="50" t="s">
-        <v>88</v>
+      <c r="C29" s="55" t="s">
+        <v>85</v>
       </c>
       <c r="D29" s="2">
         <v>0.85714285714000005</v>
@@ -4336,11 +4915,11 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="64"/>
+      <c r="A30" s="69"/>
       <c r="B30" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="50"/>
+      <c r="C30" s="55"/>
       <c r="D30" s="2">
         <v>0.83870967699999999</v>
       </c>
@@ -4373,11 +4952,11 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A31" s="65"/>
+      <c r="A31" s="70"/>
       <c r="B31" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="60"/>
+      <c r="C31" s="65"/>
       <c r="D31" s="6">
         <v>0.84444439999999998</v>
       </c>
@@ -4428,29 +5007,29 @@
       <c r="A33" s="39"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="70" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
-      <c r="J34" s="71"/>
-      <c r="K34" s="71"/>
-      <c r="L34" s="71"/>
-      <c r="M34" s="72"/>
+      <c r="A34" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="76"/>
+      <c r="M34" s="77"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="64" t="s">
-        <v>90</v>
+      <c r="A35" s="69" t="s">
+        <v>87</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>42</v>
@@ -4477,19 +5056,19 @@
         <v>49</v>
       </c>
       <c r="L35" s="26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M35" s="35" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="64"/>
+      <c r="A36" s="69"/>
       <c r="B36" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="50" t="s">
-        <v>88</v>
+      <c r="C36" s="55" t="s">
+        <v>85</v>
       </c>
       <c r="D36" s="2">
         <v>0.6</v>
@@ -4531,11 +5110,11 @@
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="64"/>
+      <c r="A37" s="69"/>
       <c r="B37" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="50"/>
+      <c r="C37" s="55"/>
       <c r="D37" s="2">
         <v>0.58394160579999999</v>
       </c>
@@ -4568,11 +5147,11 @@
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="61"/>
+      <c r="A38" s="66"/>
       <c r="B38" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="66"/>
+      <c r="C38" s="71"/>
       <c r="D38" s="44">
         <v>0.59420289000000004</v>
       </c>
@@ -4635,27 +5214,27 @@
       <c r="M40" s="1"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="70" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41" s="71"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="71"/>
-      <c r="G41" s="71"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="71"/>
-      <c r="K41" s="71"/>
-      <c r="L41" s="71"/>
-      <c r="M41" s="72"/>
+      <c r="A41" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="76"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="76"/>
+      <c r="L41" s="76"/>
+      <c r="M41" s="77"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="43"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D42" s="26" t="s">
         <v>42</v>
@@ -4682,21 +5261,21 @@
         <v>49</v>
       </c>
       <c r="L42" s="26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M42" s="35" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="64" t="s">
-        <v>90</v>
+      <c r="A43" s="69" t="s">
+        <v>87</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="50" t="s">
-        <v>88</v>
+      <c r="C43" s="55" t="s">
+        <v>85</v>
       </c>
       <c r="D43" s="2">
         <v>0.84705882349999995</v>
@@ -4738,11 +5317,11 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="64"/>
+      <c r="A44" s="69"/>
       <c r="B44" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="50"/>
+      <c r="C44" s="55"/>
       <c r="D44" s="2">
         <v>0.58394160579999999</v>
       </c>
@@ -4775,11 +5354,11 @@
       </c>
     </row>
     <row r="45" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A45" s="65"/>
+      <c r="A45" s="70"/>
       <c r="B45" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="60"/>
+      <c r="C45" s="65"/>
       <c r="D45" s="6">
         <v>0.66666666600000002</v>
       </c>
@@ -4812,27 +5391,27 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="50"/>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="50"/>
-      <c r="J48" s="50"/>
-      <c r="K48" s="50"/>
-      <c r="L48" s="50"/>
-      <c r="M48" s="50"/>
+      <c r="A48" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="55"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="55"/>
+      <c r="G48" s="55"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="55"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="55"/>
+      <c r="L48" s="55"/>
+      <c r="M48" s="55"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D49" s="26" t="s">
         <v>42</v>
@@ -4859,21 +5438,21 @@
         <v>49</v>
       </c>
       <c r="L49" s="26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="49" t="s">
-        <v>90</v>
+      <c r="A50" s="54" t="s">
+        <v>87</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="50" t="s">
-        <v>88</v>
+      <c r="C50" s="55" t="s">
+        <v>85</v>
       </c>
       <c r="D50" s="2">
         <v>0.50331125827000001</v>
@@ -4907,11 +5486,11 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="49"/>
+      <c r="A51" s="54"/>
       <c r="B51" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="50"/>
+      <c r="C51" s="55"/>
       <c r="D51" s="2">
         <v>0.58394159999999995</v>
       </c>
@@ -4944,11 +5523,11 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="49"/>
+      <c r="A52" s="54"/>
       <c r="B52" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="50"/>
+      <c r="C52" s="55"/>
       <c r="D52" s="2">
         <v>0.53608247421999999</v>
       </c>
@@ -4981,27 +5560,27 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="50"/>
-      <c r="I55" s="50"/>
-      <c r="J55" s="50"/>
-      <c r="K55" s="50"/>
-      <c r="L55" s="50"/>
-      <c r="M55" s="50"/>
+      <c r="A55" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55" s="55"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="55"/>
+      <c r="G55" s="55"/>
+      <c r="H55" s="55"/>
+      <c r="I55" s="55"/>
+      <c r="J55" s="55"/>
+      <c r="K55" s="55"/>
+      <c r="L55" s="55"/>
+      <c r="M55" s="55"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D56" s="30" t="s">
         <v>42</v>
@@ -5028,21 +5607,21 @@
         <v>49</v>
       </c>
       <c r="L56" s="30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="49" t="s">
-        <v>90</v>
+      <c r="A57" s="54" t="s">
+        <v>87</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="50" t="s">
-        <v>88</v>
+      <c r="C57" s="55" t="s">
+        <v>85</v>
       </c>
       <c r="D57" s="2">
         <v>0.42962962962962897</v>
@@ -5076,11 +5655,11 @@
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="49"/>
+      <c r="A58" s="54"/>
       <c r="B58" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C58" s="50"/>
+      <c r="C58" s="55"/>
       <c r="D58" s="2">
         <v>0.39705882352941102</v>
       </c>
@@ -5113,11 +5692,11 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="49"/>
+      <c r="A59" s="54"/>
       <c r="B59" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="50"/>
+      <c r="C59" s="55"/>
       <c r="D59" s="2">
         <v>0.434108527131782</v>
       </c>
@@ -5150,27 +5729,27 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="50" t="s">
-        <v>98</v>
-      </c>
-      <c r="B62" s="50"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="50"/>
-      <c r="E62" s="50"/>
-      <c r="F62" s="50"/>
-      <c r="G62" s="50"/>
-      <c r="H62" s="50"/>
-      <c r="I62" s="50"/>
-      <c r="J62" s="50"/>
-      <c r="K62" s="50"/>
-      <c r="L62" s="50"/>
-      <c r="M62" s="50"/>
+      <c r="A62" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="B62" s="55"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="55"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="55"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="55"/>
+      <c r="I62" s="55"/>
+      <c r="J62" s="55"/>
+      <c r="K62" s="55"/>
+      <c r="L62" s="55"/>
+      <c r="M62" s="55"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D63" s="30" t="s">
         <v>42</v>
@@ -5197,21 +5776,21 @@
         <v>49</v>
       </c>
       <c r="L63" s="30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M63" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="49" t="s">
-        <v>90</v>
+      <c r="A64" s="54" t="s">
+        <v>87</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C64" s="50" t="s">
-        <v>88</v>
+      <c r="C64" s="55" t="s">
+        <v>85</v>
       </c>
       <c r="D64" s="2">
         <v>0.875</v>
@@ -5245,11 +5824,11 @@
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="49"/>
+      <c r="A65" s="54"/>
       <c r="B65" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="50"/>
+      <c r="C65" s="55"/>
       <c r="D65" s="2">
         <v>0.81720430099999997</v>
       </c>
@@ -5282,11 +5861,11 @@
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="49"/>
+      <c r="A66" s="54"/>
       <c r="B66" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C66" s="50"/>
+      <c r="C66" s="55"/>
       <c r="D66" s="2">
         <v>0.85106382899999999</v>
       </c>
@@ -5347,4 +5926,661 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:O24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="2" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77"/>
+      <c r="N3" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="69"/>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.90109890109000002</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.88888888887999995</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.86021505369999995</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.82105263157889996</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.81632653060000004</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.85416666659999996</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.86956521730000003</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.91489361700000005</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.81318681317999997</v>
+      </c>
+      <c r="M5" s="35">
+        <v>0.86956521730000003</v>
+      </c>
+      <c r="N5">
+        <f>AVERAGE(D5:M5)</f>
+        <v>0.86089595372288996</v>
+      </c>
+      <c r="O5">
+        <f>_xlfn.STDEV.S(D5:M5)</f>
+        <v>3.5530541033785154E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="69"/>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="2">
+        <v>0.90109890109000002</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.85393258425999996</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.82222222219999996</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.82978723404200005</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.82474226803999995</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.82758620689600004</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.88888888880000005</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.89130434700000005</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.74468085106000004</v>
+      </c>
+      <c r="M6" s="35">
+        <v>0.89130434782599999</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N7" si="0">AVERAGE(D6:M6)</f>
+        <v>0.84755478512140014</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:O7" si="1">_xlfn.STDEV.S(D6:M6)</f>
+        <v>4.81938575866789E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="66"/>
+      <c r="B7" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="71"/>
+      <c r="D7" s="44">
+        <v>0.90109890109000002</v>
+      </c>
+      <c r="E7" s="44">
+        <v>0.87912087910000003</v>
+      </c>
+      <c r="F7" s="44">
+        <v>0.81318681309999996</v>
+      </c>
+      <c r="G7" s="44">
+        <v>0.83870967741900004</v>
+      </c>
+      <c r="H7" s="44">
+        <v>0.82474226803999995</v>
+      </c>
+      <c r="I7" s="44">
+        <v>0.86363636362999996</v>
+      </c>
+      <c r="J7" s="44">
+        <v>0.87912087900000002</v>
+      </c>
+      <c r="K7" s="44">
+        <v>0.90526315700000004</v>
+      </c>
+      <c r="L7" s="44">
+        <v>0.78260869565199997</v>
+      </c>
+      <c r="M7" s="45">
+        <v>0.86956521739000003</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0.8557052851421002</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>3.9814338296297144E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="40"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="10" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="77"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" s="35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="69"/>
+      <c r="B13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.80487804799999996</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.86046511599999997</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.77894736840000001</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.81720430099999997</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.80459770109999995</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.79545454545000005</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.88636363636000004</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.85416666600000002</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.76543209869999995</v>
+      </c>
+      <c r="M13" s="35">
+        <v>0.85148514851000001</v>
+      </c>
+      <c r="N13">
+        <f>AVERAGE(D13:M13)</f>
+        <v>0.82189946295199989</v>
+      </c>
+      <c r="O13">
+        <f>_xlfn.STDEV.S(D13:M13)</f>
+        <v>3.9304124494114571E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="69"/>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="55"/>
+      <c r="D14" s="2">
+        <v>0.79120879119999998</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.82105263156999997</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.74468085100000003</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.84782608695600004</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.71578947368000001</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.70588235294099999</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.75294117647049996</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.80808080800000004</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.70454545453999995</v>
+      </c>
+      <c r="M14" s="35">
+        <v>0.77272727200000002</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ref="N14:N15" si="2">AVERAGE(D14:M14)</f>
+        <v>0.76647348983575003</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ref="O14:O15" si="3">_xlfn.STDEV.S(D14:M14)</f>
+        <v>5.0235579636043519E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="66"/>
+      <c r="B15" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="71"/>
+      <c r="D15" s="44">
+        <v>0.81395348837000003</v>
+      </c>
+      <c r="E15" s="44">
+        <v>0.85714285710000004</v>
+      </c>
+      <c r="F15" s="44">
+        <v>0.80412371134000005</v>
+      </c>
+      <c r="G15" s="44">
+        <v>0.85106382977999995</v>
+      </c>
+      <c r="H15" s="44">
+        <v>0.8</v>
+      </c>
+      <c r="I15" s="44">
+        <v>0.77894736842000001</v>
+      </c>
+      <c r="J15" s="44">
+        <v>0.82978723403999999</v>
+      </c>
+      <c r="K15" s="44">
+        <v>0.909090909</v>
+      </c>
+      <c r="L15" s="44">
+        <v>0.72727272700000001</v>
+      </c>
+      <c r="M15" s="45">
+        <v>0.84444443999999996</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>0.82158265650499995</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="3"/>
+        <v>4.9353935522131437E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="46"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="46"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="20" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J21" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L21" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="71" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.90526315789</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.85714285710000004</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.84536082473999996</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.82474226803999995</v>
+      </c>
+      <c r="H22" s="18">
+        <v>0.80898876399999997</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.86363636300000002</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.86956521730000003</v>
+      </c>
+      <c r="K22" s="18">
+        <v>0.92473117999999999</v>
+      </c>
+      <c r="L22" s="18">
+        <v>0.79120879119999998</v>
+      </c>
+      <c r="M22" s="38">
+        <v>0.869565217</v>
+      </c>
+      <c r="N22">
+        <f>AVERAGE(D22:M22)</f>
+        <v>0.85602046402700016</v>
+      </c>
+      <c r="O22">
+        <f>_xlfn.STDEV.S(D22:M22)</f>
+        <v>4.0929037426725483E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="81"/>
+      <c r="B23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="78"/>
+      <c r="D23" s="2">
+        <v>0.89361702119999997</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.83720930232000002</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.80952380950000002</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.83870967741000002</v>
+      </c>
+      <c r="H23" s="38">
+        <v>0.81632653060000004</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0.83720930232500002</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.87640449438000001</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0.86315788999999998</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.76744186039999995</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.89130434780000001</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ref="N23:N24" si="4">AVERAGE(D23:M23)</f>
+        <v>0.84309042359349995</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ref="O23:O24" si="5">_xlfn.STDEV.S(D23:M23)</f>
+        <v>3.9502664957170697E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="82"/>
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="79"/>
+      <c r="D24" s="2">
+        <v>0.89361702119999997</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.84782608694999995</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.82352941176399996</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.83870967741000002</v>
+      </c>
+      <c r="H24" s="38">
+        <v>0.83673469300000003</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.86021505375999996</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.87912087910000003</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.91489359999999997</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.79120879119999998</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0.86021505300000001</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="4"/>
+        <v>0.85460702673839994</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="5"/>
+        <v>3.5626708242820944E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A11:M11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="C13:C15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>